<commit_message>
Update do doc de auto-avaliação
</commit_message>
<xml_diff>
--- a/Documentacao/Entrega 2/Autoavaliação/Autoavaliação TP2 - Grupo 1.xlsx
+++ b/Documentacao/Entrega 2/Autoavaliação/Autoavaliação TP2 - Grupo 1.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18625"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20520" windowHeight="11076"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20520" windowHeight="11080"/>
   </bookViews>
   <sheets>
     <sheet name="Avaliação" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="61">
   <si>
     <t>Peso</t>
   </si>
@@ -88,18 +88,6 @@
     <t>Individual</t>
   </si>
   <si>
-    <t>Nr. aluno 1</t>
-  </si>
-  <si>
-    <t>Nr. aluno 2</t>
-  </si>
-  <si>
-    <t>Nr. aluno 3</t>
-  </si>
-  <si>
-    <t>Nr. aluno 5</t>
-  </si>
-  <si>
     <t>Existe um registo regular da sua atividade no bitbucket  (individual)</t>
   </si>
   <si>
@@ -214,16 +202,16 @@
     <t>Manuel Correira</t>
   </si>
   <si>
-    <t>Daniel Bento</t>
-  </si>
-  <si>
     <t>Carolina Barros</t>
+  </si>
+  <si>
+    <t>Daniel    Bento</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -321,7 +309,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -343,7 +331,6 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -351,6 +338,12 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -648,21 +641,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J42"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E23" sqref="E23"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="H18" sqref="H18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="3" max="3" width="71.44140625" customWidth="1"/>
-    <col min="4" max="4" width="12.109375" customWidth="1"/>
-    <col min="5" max="9" width="11.44140625" customWidth="1"/>
+    <col min="3" max="3" width="71.453125" customWidth="1"/>
+    <col min="4" max="4" width="12.08984375" customWidth="1"/>
+    <col min="5" max="9" width="11.453125" customWidth="1"/>
     <col min="10" max="10" width="102" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>19</v>
@@ -671,41 +664,41 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="E2" s="10" t="s">
-        <v>64</v>
-      </c>
-      <c r="F2" s="10" t="s">
-        <v>63</v>
-      </c>
-      <c r="G2" s="10" t="s">
-        <v>62</v>
-      </c>
-      <c r="H2" s="10" t="s">
-        <v>61</v>
-      </c>
-      <c r="I2" s="10" t="s">
+    <row r="2" spans="1:10" ht="29" x14ac:dyDescent="0.35">
+      <c r="E2" s="19" t="s">
+        <v>59</v>
+      </c>
+      <c r="F2" s="19" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="E3" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="F3" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="G3" s="11" t="s">
-        <v>23</v>
-      </c>
-      <c r="H3" s="11">
+      <c r="G2" s="19" t="s">
+        <v>58</v>
+      </c>
+      <c r="H2" s="19" t="s">
+        <v>57</v>
+      </c>
+      <c r="I2" s="19" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="E3" s="18">
+        <v>1121107</v>
+      </c>
+      <c r="F3" s="18">
+        <v>1101516</v>
+      </c>
+      <c r="G3" s="18">
+        <v>1120557</v>
+      </c>
+      <c r="H3" s="18">
         <v>1120569</v>
       </c>
-      <c r="I3" s="11" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="I3" s="18">
+        <v>1130739</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>0</v>
       </c>
@@ -717,113 +710,137 @@
         <v>18</v>
       </c>
       <c r="J4" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A5" s="3">
         <v>0.1</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C5" s="5"/>
       <c r="D5" s="5"/>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
       <c r="C6" t="s">
-        <v>36</v>
-      </c>
-      <c r="E6" s="18" t="s">
-        <v>49</v>
-      </c>
-      <c r="F6" s="18"/>
-      <c r="G6" s="18"/>
-      <c r="H6" s="18" t="s">
-        <v>45</v>
-      </c>
-      <c r="I6" s="18"/>
-      <c r="J6" s="12"/>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+        <v>32</v>
+      </c>
+      <c r="E6" s="17" t="s">
+        <v>41</v>
+      </c>
+      <c r="F6" s="17"/>
+      <c r="G6" s="17" t="s">
+        <v>41</v>
+      </c>
+      <c r="H6" s="17" t="s">
+        <v>41</v>
+      </c>
+      <c r="I6" s="17" t="s">
+        <v>41</v>
+      </c>
+      <c r="J6" s="11"/>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
       <c r="C7" t="s">
-        <v>37</v>
-      </c>
-      <c r="E7" s="18" t="s">
-        <v>49</v>
-      </c>
-      <c r="F7" s="18"/>
-      <c r="G7" s="18"/>
-      <c r="H7" s="18" t="s">
-        <v>45</v>
-      </c>
-      <c r="I7" s="18"/>
-      <c r="J7" s="12"/>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+        <v>33</v>
+      </c>
+      <c r="E7" s="17" t="s">
+        <v>41</v>
+      </c>
+      <c r="F7" s="17" t="s">
+        <v>45</v>
+      </c>
+      <c r="G7" s="17" t="s">
+        <v>41</v>
+      </c>
+      <c r="H7" s="17" t="s">
+        <v>41</v>
+      </c>
+      <c r="I7" s="17" t="s">
+        <v>41</v>
+      </c>
+      <c r="J7" s="11"/>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
       <c r="C8" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="E8" s="18" t="s">
-        <v>45</v>
-      </c>
-      <c r="F8" s="18"/>
-      <c r="G8" s="18"/>
-      <c r="H8" s="18" t="s">
-        <v>45</v>
-      </c>
-      <c r="I8" s="18"/>
-      <c r="J8" s="12"/>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+        <v>21</v>
+      </c>
+      <c r="E8" s="17" t="s">
+        <v>41</v>
+      </c>
+      <c r="F8" s="17"/>
+      <c r="G8" s="17" t="s">
+        <v>41</v>
+      </c>
+      <c r="H8" s="17" t="s">
+        <v>41</v>
+      </c>
+      <c r="I8" s="17" t="s">
+        <v>41</v>
+      </c>
+      <c r="J8" s="11"/>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
       <c r="C9" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="E9" s="18" t="s">
-        <v>45</v>
-      </c>
-      <c r="F9" s="18"/>
-      <c r="G9" s="18"/>
-      <c r="H9" s="18" t="s">
-        <v>45</v>
-      </c>
-      <c r="I9" s="18"/>
-      <c r="J9" s="12"/>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+        <v>35</v>
+      </c>
+      <c r="E9" s="17" t="s">
+        <v>45</v>
+      </c>
+      <c r="F9" s="17"/>
+      <c r="G9" s="17" t="s">
+        <v>45</v>
+      </c>
+      <c r="H9" s="17" t="s">
+        <v>45</v>
+      </c>
+      <c r="I9" s="17" t="s">
+        <v>45</v>
+      </c>
+      <c r="J9" s="11"/>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
       <c r="C10" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="D10" s="18"/>
-      <c r="J10" s="12"/>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+        <v>22</v>
+      </c>
+      <c r="D10" s="17" t="s">
+        <v>51</v>
+      </c>
+      <c r="J10" s="11"/>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
       <c r="C11" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="D11" s="18"/>
-      <c r="J11" s="12"/>
-    </row>
-    <row r="12" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="D11" s="17" t="s">
+        <v>41</v>
+      </c>
+      <c r="J11" s="11"/>
+    </row>
+    <row r="12" spans="1:10" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A12" s="3">
         <v>0.05</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="C12" s="4"/>
       <c r="D12" s="5"/>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A13" s="8"/>
       <c r="B13" s="8"/>
       <c r="C13" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="D13" s="18"/>
-      <c r="J13" s="12"/>
-    </row>
-    <row r="15" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="D13" s="17" t="s">
+        <v>51</v>
+      </c>
+      <c r="J13" s="11"/>
+    </row>
+    <row r="15" spans="1:10" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A15" s="3">
         <v>0.25</v>
       </c>
@@ -833,32 +850,36 @@
       <c r="C15" s="4"/>
       <c r="D15" s="5"/>
     </row>
-    <row r="16" spans="1:10" ht="31.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:10" ht="31.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16" s="8"/>
       <c r="B16" s="8"/>
       <c r="C16" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="D16" s="14"/>
-      <c r="J16" s="12"/>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="D16" s="13"/>
+      <c r="J16" s="11"/>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.35">
       <c r="C17" t="s">
         <v>6</v>
       </c>
-      <c r="D17" s="18"/>
-      <c r="J17" s="12"/>
-    </row>
-    <row r="18" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="D17" s="17" t="s">
+        <v>51</v>
+      </c>
+      <c r="J17" s="11"/>
+    </row>
+    <row r="18" spans="1:10" ht="29" x14ac:dyDescent="0.35">
       <c r="C18" s="9" t="s">
-        <v>34</v>
-      </c>
-      <c r="D18" s="18"/>
-      <c r="J18" s="12" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
+        <v>30</v>
+      </c>
+      <c r="D18" s="17" t="s">
+        <v>51</v>
+      </c>
+      <c r="J18" s="11" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A19" s="3">
         <v>0.4</v>
       </c>
@@ -868,50 +889,58 @@
       <c r="C19" s="4"/>
       <c r="D19" s="5"/>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.35">
       <c r="C20" t="s">
         <v>8</v>
       </c>
-      <c r="D20" s="18"/>
-      <c r="J20" s="12"/>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="D20" s="17" t="s">
+        <v>45</v>
+      </c>
+      <c r="J20" s="11"/>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.35">
       <c r="C21" t="s">
         <v>9</v>
       </c>
-      <c r="D21" s="18"/>
-      <c r="J21" s="12"/>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="D21" s="17" t="s">
+        <v>45</v>
+      </c>
+      <c r="J21" s="11"/>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.35">
       <c r="C22" t="s">
         <v>10</v>
       </c>
-      <c r="D22" s="14"/>
-      <c r="J22" s="12"/>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="D22" s="13"/>
+      <c r="J22" s="11"/>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.35">
       <c r="C23" t="s">
-        <v>43</v>
-      </c>
-      <c r="E23" s="18" t="s">
-        <v>49</v>
-      </c>
-      <c r="F23" s="18"/>
-      <c r="G23" s="18"/>
-      <c r="H23" s="18" t="s">
-        <v>49</v>
-      </c>
-      <c r="I23" s="18"/>
-      <c r="J23" s="12"/>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
+        <v>39</v>
+      </c>
+      <c r="E23" s="17" t="s">
+        <v>45</v>
+      </c>
+      <c r="F23" s="17"/>
+      <c r="G23" s="17" t="s">
+        <v>45</v>
+      </c>
+      <c r="H23" s="17" t="s">
+        <v>45</v>
+      </c>
+      <c r="I23" s="17" t="s">
+        <v>45</v>
+      </c>
+      <c r="J23" s="11"/>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.35">
       <c r="C24" t="s">
-        <v>38</v>
-      </c>
-      <c r="D24" s="14"/>
-      <c r="J24" s="12"/>
-    </row>
-    <row r="25" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
+        <v>34</v>
+      </c>
+      <c r="D24" s="13"/>
+      <c r="J24" s="11"/>
+    </row>
+    <row r="25" spans="1:10" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A25" s="3">
         <v>0.1</v>
       </c>
@@ -921,24 +950,26 @@
       <c r="C25" s="4"/>
       <c r="D25" s="5"/>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.35">
       <c r="C26" t="s">
         <v>12</v>
       </c>
-      <c r="D26" s="18"/>
-      <c r="J26" s="12"/>
-    </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="D26" s="17" t="s">
+        <v>45</v>
+      </c>
+      <c r="J26" s="11"/>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.35">
       <c r="C27" t="s">
         <v>13</v>
       </c>
-      <c r="D27" s="14"/>
-      <c r="J27" s="12"/>
-    </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="J28" s="12"/>
-    </row>
-    <row r="29" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="D27" s="13"/>
+      <c r="J27" s="11"/>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="J28" s="11"/>
+    </row>
+    <row r="29" spans="1:10" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A29" s="3">
         <v>0.1</v>
       </c>
@@ -948,82 +979,82 @@
       <c r="C29" s="4"/>
       <c r="D29" s="5"/>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.35">
       <c r="C30" t="s">
         <v>15</v>
       </c>
-      <c r="D30" s="16" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="D30" s="15" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.35">
       <c r="C31" t="s">
         <v>16</v>
       </c>
-      <c r="D31" s="16" t="s">
-        <v>30</v>
-      </c>
-      <c r="F31" s="17"/>
-    </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="D31" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="F31" s="16"/>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.35">
       <c r="C32" t="s">
         <v>17</v>
       </c>
-      <c r="D32" s="16" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D32" s="15" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.35">
       <c r="C33" t="s">
-        <v>42</v>
-      </c>
-      <c r="D33" s="16" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+        <v>38</v>
+      </c>
+      <c r="D33" s="15" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.35">
       <c r="C34" t="s">
-        <v>29</v>
-      </c>
-      <c r="D34" s="16" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
+        <v>25</v>
+      </c>
+      <c r="D34" s="15" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A35" s="3"/>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A36" s="15"/>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A36" s="14"/>
       <c r="B36" s="1"/>
       <c r="C36" s="1"/>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A38" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B39" s="2"/>
       <c r="C39" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B40" s="10"/>
       <c r="C40" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B41" s="11"/>
+      <c r="C41" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B41" s="12"/>
-      <c r="C41" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B42" s="13"/>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B42" s="12"/>
       <c r="C42" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
     </row>
   </sheetData>
@@ -1034,7 +1065,7 @@
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
-            <xm:f>[1]Sheet2!#REF!</xm:f>
+            <xm:f>'C:\TudoPortatil\ISEP\BD\2017-2018\[BDDAD_Avaliação_TP_Parte2_AJO.xlsx]Sheet2'!#REF!</xm:f>
           </x14:formula1>
           <xm:sqref>F31</xm:sqref>
         </x14:dataValidation>
@@ -1055,90 +1086,90 @@
   <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="14.44140625" customWidth="1"/>
-    <col min="4" max="4" width="63.88671875" customWidth="1"/>
+    <col min="1" max="1" width="14.453125" customWidth="1"/>
+    <col min="4" max="4" width="63.90625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="B1">
         <v>0</v>
       </c>
       <c r="D1" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="B2">
         <v>0.2</v>
       </c>
       <c r="D2" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="B3">
         <v>0.4</v>
       </c>
       <c r="D3" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="B4">
         <v>0.6</v>
       </c>
       <c r="D4" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="B5">
         <v>0.75</v>
       </c>
       <c r="D5" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="B6">
         <v>0.85</v>
       </c>
       <c r="D6" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="B7">
         <v>1</v>
       </c>
       <c r="D7" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
     </row>
   </sheetData>

</xml_diff>